<commit_message>
2.2.2 Upgraded Bank Account imports
</commit_message>
<xml_diff>
--- a/bank_accounts.xlsx
+++ b/bank_accounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gst-invoicer-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8715D63-2CAF-4BB8-A430-77455122BB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D882F194-BF60-485D-BC6D-FD10F32A2E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{794B317B-B4F9-46A2-9BD9-5B4D1E130541}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Currency</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>Chembur Central Avenue</t>
+  </si>
+  <si>
+    <t>Kotak Mahindra Bank</t>
+  </si>
+  <si>
+    <t>KKBK0001477</t>
+  </si>
+  <si>
+    <t>KKBKINBB</t>
+  </si>
+  <si>
+    <t>Wadala Branch</t>
   </si>
 </sst>
 </file>
@@ -465,13 +477,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEFB8067-F379-4B15-A13B-E05897934945}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -551,6 +566,26 @@
       </c>
       <c r="F4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>9769689780</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>